<commit_message>
Dictionnaire des données cas Horse1
</commit_message>
<xml_diff>
--- a/DictionnaireDonnees.xlsx
+++ b/DictionnaireDonnees.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER-3\Desktop\CDA2024-2025\CDA23016_TP JAVA Base de donnees\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER-3\Desktop\CDA2024-2025\Essais github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674450A7-15F0-4CBB-98D3-45EC6E46AF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0B30C-580A-4545-86A8-4A34AB1824E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{40451DEB-308C-4DBD-9635-497D12915BC3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{40451DEB-308C-4DBD-9635-497D12915BC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CasVideo" sheetId="1" r:id="rId1"/>
@@ -178,9 +178,6 @@
     <t xml:space="preserve">1,N </t>
   </si>
   <si>
-    <t>CURRENCY</t>
-  </si>
-  <si>
     <t>DICTIONNAIRE DES DONNEES CAS VIDEO</t>
   </si>
   <si>
@@ -521,6 +518,9 @@
   </si>
   <si>
     <t>Type/JockeyDriver/Course</t>
+  </si>
+  <si>
+    <t>NUMERIQUE</t>
   </si>
 </sst>
 </file>
@@ -689,6 +689,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -698,8 +701,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -709,15 +718,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1038,8 +1038,8 @@
   </sheetPr>
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,39 +1056,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
+      <c r="A1" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="11"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="4" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="5" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="6" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="7" spans="1:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="8" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="9" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="10" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="11" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>13</v>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="12" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>12</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="13" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>12</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="14" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="15" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>17</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="16" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>13</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="17" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>19</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="18" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>12</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="19" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
@@ -1623,13 +1623,13 @@
     </row>
     <row r="21" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
@@ -1651,13 +1651,13 @@
     </row>
     <row r="22" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
@@ -1679,7 +1679,7 @@
     </row>
     <row r="23" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>13</v>
@@ -1709,7 +1709,7 @@
     </row>
     <row r="24" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>13</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="25" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>12</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="26" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>13</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="27" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="28" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>12</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="29" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>12</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="30" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>12</v>
@@ -1905,7 +1905,7 @@
     </row>
     <row r="31" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>12</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="32" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>12</v>
@@ -1959,7 +1959,7 @@
     </row>
     <row r="33" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>12</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="34" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>13</v>
@@ -2015,7 +2015,7 @@
     </row>
     <row r="35" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>12</v>
@@ -2043,7 +2043,7 @@
     </row>
     <row r="36" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>13</v>
@@ -2071,7 +2071,7 @@
     </row>
     <row r="37" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>17</v>
@@ -2097,7 +2097,7 @@
     </row>
     <row r="38" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>17</v>
@@ -2123,10 +2123,10 @@
     </row>
     <row r="39" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>50</v>
+        <v>164</v>
       </c>
       <c r="C39" s="9">
         <v>2</v>
@@ -2163,7 +2163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8D9B80-FBC0-43E6-9CB0-1F08BBEABE34}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
@@ -2178,39 +2178,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17"/>
+      <c r="A1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="11"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2240,8 +2240,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>53</v>
+      <c r="A4" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>13</v>
@@ -2257,21 +2257,21 @@
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>25</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>12</v>
@@ -2291,15 +2291,15 @@
         <v>25</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -2315,21 +2315,21 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
@@ -2349,15 +2349,15 @@
         <v>25</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
@@ -2377,15 +2377,15 @@
         <v>25</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -2405,15 +2405,15 @@
         <v>25</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -2435,15 +2435,15 @@
         <v>25</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -2463,15 +2463,15 @@
         <v>25</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>13</v>
@@ -2487,21 +2487,21 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>12</v>
@@ -2521,15 +2521,15 @@
         <v>25</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -2545,21 +2545,21 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -2579,15 +2579,15 @@
         <v>25</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>13</v>
@@ -2603,21 +2603,21 @@
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>13</v>
@@ -2639,15 +2639,15 @@
         <v>25</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>13</v>
@@ -2663,21 +2663,21 @@
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H18" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="I18" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="J18" s="9" t="s">
         <v>148</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>12</v>
@@ -2697,15 +2697,15 @@
         <v>25</v>
       </c>
       <c r="I19" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="J19" s="9" t="s">
         <v>148</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
@@ -2721,21 +2721,21 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
@@ -2755,15 +2755,15 @@
         <v>25</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>13</v>
@@ -2779,21 +2779,21 @@
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>25</v>
       </c>
       <c r="I22" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>13</v>
@@ -2815,15 +2815,15 @@
         <v>25</v>
       </c>
       <c r="I23" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J23" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>17</v>
@@ -2843,15 +2843,15 @@
         <v>25</v>
       </c>
       <c r="I24" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>12</v>
@@ -2871,15 +2871,15 @@
         <v>25</v>
       </c>
       <c r="I25" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>12</v>
@@ -2899,15 +2899,15 @@
         <v>25</v>
       </c>
       <c r="I26" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>12</v>
@@ -2927,15 +2927,15 @@
         <v>25</v>
       </c>
       <c r="I27" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J27" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>12</v>
@@ -2955,15 +2955,15 @@
         <v>25</v>
       </c>
       <c r="I28" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J28" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>19</v>
@@ -2983,15 +2983,15 @@
         <v>25</v>
       </c>
       <c r="I29" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J29" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>12</v>
@@ -3011,15 +3011,15 @@
         <v>25</v>
       </c>
       <c r="I30" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J30" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>12</v>
@@ -3039,15 +3039,15 @@
         <v>25</v>
       </c>
       <c r="I31" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J31" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>13</v>
@@ -3063,21 +3063,21 @@
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>12</v>
@@ -3097,15 +3097,15 @@
         <v>25</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>13</v>
@@ -3121,21 +3121,21 @@
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>25</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>12</v>
@@ -3155,15 +3155,15 @@
         <v>25</v>
       </c>
       <c r="I35" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="J35" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>17</v>
@@ -3183,15 +3183,15 @@
         <v>25</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>13</v>
@@ -3207,21 +3207,21 @@
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
@@ -3243,15 +3243,15 @@
         <v>25</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
@@ -3271,15 +3271,15 @@
         <v>25</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>12</v>
@@ -3299,15 +3299,15 @@
         <v>25</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>12</v>
@@ -3327,15 +3327,15 @@
         <v>25</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>12</v>
@@ -3349,24 +3349,24 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C43" s="1">
         <v>4</v>
@@ -3377,21 +3377,21 @@
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J43" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>13</v>
@@ -3407,21 +3407,21 @@
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>25</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>13</v>
@@ -3441,15 +3441,15 @@
         <v>25</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>12</v>
@@ -3469,15 +3469,15 @@
         <v>25</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>13</v>
@@ -3497,15 +3497,15 @@
         <v>25</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>12</v>
@@ -3525,15 +3525,15 @@
         <v>25</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J48" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>12</v>
@@ -3553,15 +3553,15 @@
         <v>25</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>12</v>
@@ -3581,15 +3581,15 @@
         <v>25</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>13</v>
@@ -3605,21 +3605,21 @@
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>12</v>
@@ -3639,15 +3639,15 @@
         <v>25</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>12</v>
@@ -3667,15 +3667,15 @@
         <v>25</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>13</v>
@@ -3689,21 +3689,21 @@
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J54" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I54" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="J54" s="9" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>12</v>
@@ -3723,10 +3723,10 @@
         <v>25</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>